<commit_message>
AutoCommit_9 января 2024 г. 11:27:27_SibNout2023
</commit_message>
<xml_diff>
--- a/2023-2024_2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2023-2024_2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -164,12 +164,24 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -199,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -208,6 +220,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -518,7 +532,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -537,81 +551,83 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="4">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>3</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
-      <c r="D3">
-        <f>SUM(D4:D33)</f>
+      <c r="D3" s="5">
+        <f>SUM(D4:D50)</f>
         <v>29</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <f>SUM(F3:I3)</f>
         <v>29</v>
       </c>
-      <c r="F3">
-        <f>SUM(F4:F33)</f>
+      <c r="F3" s="5">
+        <f>SUM(F4:F50)</f>
         <v>26</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:I3" si="0">SUM(G4:G33)</f>
+      <c r="G3" s="5">
+        <f>SUM(G4:G50)</f>
         <v>2</v>
       </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="H3" s="5">
+        <f>SUM(H4:H50)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <f>SUM(I4:I50)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <f>SUM(J4:J50)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
         <f>(F2*F3+G2*G3+H2*H3+I2*I3)/E3</f>
         <v>4.8620689655172411</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <f>100*(F3+G3)/D3</f>
         <v>96.551724137931032</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="5">
         <f>100*(F3+G3+H3)/D3</f>
         <v>100</v>
       </c>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="17" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -631,15 +647,15 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:I19" si="1">IF(G$2=$C4,1,0)</f>
+        <f t="shared" ref="G4:I19" si="0">IF(G$2=$C4,1,0)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -657,19 +673,19 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:I33" si="2">IF(F$2=$C5,1,0)</f>
+        <f t="shared" ref="F5:I33" si="1">IF(F$2=$C5,1,0)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -687,19 +703,19 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -717,19 +733,19 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -747,19 +763,19 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -777,19 +793,19 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -807,19 +823,19 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -837,19 +853,19 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -867,19 +883,19 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -897,19 +913,19 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -927,19 +943,19 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -957,19 +973,19 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -987,19 +1003,19 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1017,19 +1033,19 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1047,19 +1063,19 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1077,19 +1093,19 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1107,19 +1123,19 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1137,19 +1153,19 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1167,19 +1183,19 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1197,19 +1213,19 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1227,19 +1243,19 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1257,19 +1273,19 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1287,19 +1303,19 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1317,19 +1333,19 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1347,19 +1363,19 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1377,19 +1393,19 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1407,19 +1423,19 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1437,19 +1453,19 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1467,19 +1483,19 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1497,19 +1513,19 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_9 января 2024 г. 11:31:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2023-2024_2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2023-2024_2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -532,7 +532,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:I19" si="0">IF(G$2=$C4,1,0)</f>
+        <f t="shared" ref="G4:J19" si="0">IF(G$2=$C4,1,0)</f>
         <v>0</v>
       </c>
       <c r="H4">
@@ -655,6 +655,10 @@
         <v>0</v>
       </c>
       <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -673,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:I33" si="1">IF(F$2=$C5,1,0)</f>
+        <f t="shared" ref="F5:J33" si="1">IF(F$2=$C5,1,0)</f>
         <v>0</v>
       </c>
       <c r="G5">
@@ -685,6 +689,10 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -718,6 +726,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -748,6 +760,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -775,6 +791,10 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -808,6 +828,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -838,6 +862,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -868,6 +896,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -898,6 +930,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -928,6 +964,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -958,6 +998,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -988,6 +1032,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1018,8 +1066,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1048,8 +1100,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1078,8 +1134,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1108,8 +1168,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1138,8 +1202,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1168,8 +1236,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1198,8 +1270,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1228,8 +1304,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1258,8 +1338,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1288,8 +1372,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1318,8 +1406,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1348,8 +1440,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1378,8 +1474,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1408,8 +1508,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1438,8 +1542,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1468,8 +1576,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1498,8 +1610,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -1528,8 +1644,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>